<commit_message>
Post pres results commit
</commit_message>
<xml_diff>
--- a/Additional/simulation_data.xlsx
+++ b/Additional/simulation_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\Downloads\CroziersParadox\Additional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lchauhan\Downloads\CroziersParadox-main\Additional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60EDDAC-C024-4227-AA5A-ABAB1308195B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B0783C-DF3B-42CC-8482-3970B68E1C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Folder Name</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>JobID</t>
+  </si>
+  <si>
+    <t>20240719_MutationStrengthLargerRange</t>
+  </si>
+  <si>
+    <t>20240722_ExpParam</t>
+  </si>
+  <si>
+    <t>20240723_ConstantFood</t>
+  </si>
+  <si>
+    <t>20240723_FracKilledLargerRange</t>
+  </si>
+  <si>
+    <t>20240723_MetabolicCostLargerRange</t>
+  </si>
+  <si>
+    <t>20240724_ExpParam_LowerRange</t>
   </si>
 </sst>
 </file>
@@ -395,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" customWidth="1"/>
     <col min="2" max="2" width="46.109375" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
@@ -460,6 +478,36 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>